<commit_message>
Update to tile production
</commit_message>
<xml_diff>
--- a/imporium-cards/res/imporium_lab_cards.xlsx
+++ b/imporium-cards/res/imporium_lab_cards.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5683A4F-57B2-44DC-925A-174982C1542D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1612CE58-D7B6-4274-BBDA-A1F642405FC4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20205" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20208" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="97">
   <si>
     <t>Starting_Qty</t>
   </si>
@@ -101,9 +101,6 @@
   </si>
   <si>
     <t>One copy of the imp goes to each discharge</t>
-  </si>
-  <si>
-    <t>Discard the imp and trash this card to discard an opponent's lab component</t>
   </si>
   <si>
     <t>+2 Credits OR
@@ -118,10 +115,6 @@
   <si>
     <t>+1 Buy
 +1 Imp</t>
-  </si>
-  <si>
-    <t>+1 Dispenser
-+1 Buy</t>
   </si>
   <si>
     <t>+2 Credits</t>
@@ -174,9 +167,6 @@
     <t>play</t>
   </si>
   <si>
-    <t>discard</t>
-  </si>
-  <si>
     <t>Qty</t>
   </si>
   <si>
@@ -247,10 +237,6 @@
   </si>
   <si>
     <t>.\res\graphics\Adv_Combiner.png</t>
-  </si>
-  <si>
-    <t>+2 Imp
-+1 Dispenser</t>
   </si>
   <si>
     <t>+1 Buy</t>
@@ -265,10 +251,6 @@
   </si>
   <si>
     <t>Player selects the colour of the imp leaving the converter</t>
-  </si>
-  <si>
-    <t>+3 Imps
-+1 Dispenser</t>
   </si>
   <si>
     <t>+1 Credit
@@ -311,33 +293,44 @@
 +1 Stamina</t>
   </si>
   <si>
-    <t>+1 Dispenser AND
-+1 Recipe OR
+    <t>Discard the imp and trash this card to immediately gain another with cost less than or equal to 5</t>
+  </si>
+  <si>
+    <t>The imp may move through the next machine component without activating it if the player wishes</t>
+  </si>
+  <si>
+    <t>Splice</t>
+  </si>
+  <si>
+    <t>Discard the imp and trash this card immediately</t>
+  </si>
+  <si>
+    <t>-1 Sell</t>
+  </si>
+  <si>
+    <t>-1 Credit</t>
+  </si>
+  <si>
+    <t>Pile Of Junk</t>
+  </si>
+  <si>
+    <t>Crossover Tubes</t>
+  </si>
+  <si>
+    <t>recycle</t>
+  </si>
+  <si>
+    <t>Discard the imp and trash this card to discard an opponent's lab component and give them a Pile Of Junk</t>
+  </si>
+  <si>
+    <t>+2 Imp</t>
+  </si>
+  <si>
+    <t>+1 Recipe OR
 +1 Sell</t>
   </si>
   <si>
-    <t>Discard the imp and trash this card to immediately gain another with cost less than or equal to 5</t>
-  </si>
-  <si>
-    <t>The imp may move through the next machine component without activating it if the player wishes</t>
-  </si>
-  <si>
-    <t>Splice</t>
-  </si>
-  <si>
-    <t>Discard the imp and trash this card immediately</t>
-  </si>
-  <si>
-    <t>-1 Sell</t>
-  </si>
-  <si>
-    <t>-1 Credit</t>
-  </si>
-  <si>
-    <t>Pile Of Junk</t>
-  </si>
-  <si>
-    <t>Crossover Tubes</t>
+    <t>+3 Imps</t>
   </si>
 </sst>
 </file>
@@ -704,47 +697,47 @@
   </sheetPr>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="62.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="73.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="12" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" customWidth="1"/>
+    <col min="3" max="3" width="45.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="62.5546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="73.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" customWidth="1"/>
+    <col min="9" max="12" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="100.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>0</v>
@@ -756,10 +749,10 @@
         <v>18</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -770,16 +763,16 @@
         <v>11</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H2" s="8">
         <v>8</v>
@@ -797,7 +790,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -806,16 +799,16 @@
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H3" s="7">
         <v>8</v>
@@ -831,7 +824,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -840,16 +833,16 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H4" s="7">
         <v>8</v>
@@ -865,7 +858,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -876,14 +869,14 @@
         <v>26</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="H5" s="8">
         <v>8</v>
@@ -901,7 +894,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -912,14 +905,14 @@
         <v>26</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="H6" s="8">
         <v>8</v>
@@ -937,7 +930,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -946,16 +939,16 @@
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H7" s="7">
         <v>8</v>
@@ -973,7 +966,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -982,16 +975,16 @@
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H8" s="7">
         <v>8</v>
@@ -1009,7 +1002,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1020,16 +1013,16 @@
         <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H9" s="4">
         <v>8</v>
@@ -1047,7 +1040,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1058,16 +1051,16 @@
         <v>25</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H10" s="7">
         <v>8</v>
@@ -1085,7 +1078,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1093,17 +1086,17 @@
         <v>4</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H11" s="8">
         <v>8</v>
@@ -1121,7 +1114,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
@@ -1129,17 +1122,17 @@
         <v>4</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H12" s="8">
         <v>8</v>
@@ -1157,7 +1150,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
@@ -1168,16 +1161,16 @@
         <v>24</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H13" s="4">
         <v>8</v>
@@ -1195,7 +1188,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -1206,16 +1199,16 @@
         <v>11</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H14" s="8">
         <v>8</v>
@@ -1233,7 +1226,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
@@ -1244,16 +1237,16 @@
         <v>26</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H15" s="8">
         <v>8</v>
@@ -1271,7 +1264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
@@ -1282,16 +1275,16 @@
         <v>25</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H16" s="7">
         <v>8</v>
@@ -1309,7 +1302,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
@@ -1317,19 +1310,19 @@
         <v>4</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H17" s="8">
         <v>8</v>
@@ -1347,7 +1340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
@@ -1355,19 +1348,19 @@
         <v>4</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H18" s="8">
         <v>8</v>
@@ -1385,25 +1378,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B19" s="4">
         <v>3</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H19" s="7">
         <v>8</v>
@@ -1421,25 +1414,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B20" s="4">
         <v>3</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H20" s="7">
         <v>8</v>
@@ -1457,7 +1450,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
@@ -1465,19 +1458,19 @@
         <v>3</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H21" s="5">
         <v>8</v>
@@ -1495,7 +1488,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
@@ -1503,19 +1496,19 @@
         <v>2</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H22" s="7">
         <v>8</v>
@@ -1533,7 +1526,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -1542,16 +1535,16 @@
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H23" s="5">
         <v>8</v>
@@ -1569,25 +1562,25 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B24" s="4">
         <v>-1</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H24" s="5">
         <v>8</v>
@@ -1605,9 +1598,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B25" s="4">
         <v>2</v>
@@ -1618,10 +1611,10 @@
         <v>3</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H25" s="5">
         <v>8</v>
@@ -1639,16 +1632,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="M27" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="N27">
         <f>SUM(L2:L26)</f>
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="N28">
         <f>N27/12</f>
         <v>16</v>

</xml_diff>